<commit_message>
Starting work on full Jail PM file
</commit_message>
<xml_diff>
--- a/CDC Vital Population Statisitics/Jail_PM/Jail PM Data/sjc_site_populations_jail_pm_2010_2020.xlsx
+++ b/CDC Vital Population Statisitics/Jail_PM/Jail PM Data/sjc_site_populations_jail_pm_2010_2020.xlsx
@@ -32,37 +32,37 @@
     <t xml:space="preserve">pop_adult_male_any_ethnicity</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_adult_femlae_any_ethnicity</t>
+    <t xml:space="preserve">pop_adult_female_any_ethnicity</t>
   </si>
   <si>
-    <t xml:space="preserve">total_pop_young_any_ethnicity</t>
+    <t xml:space="preserve">pop_young_any_ethnicity</t>
   </si>
   <si>
-    <t xml:space="preserve">total_pop_middle_any_ethnicity</t>
+    <t xml:space="preserve">pop_middle_any_ethnicity</t>
   </si>
   <si>
-    <t xml:space="preserve">total_pop_older_any_ethnicity</t>
+    <t xml:space="preserve">pop_older_any_ethnicity</t>
   </si>
   <si>
-    <t xml:space="preserve">total_pop_poc</t>
+    <t xml:space="preserve">pop_total_poc</t>
   </si>
   <si>
-    <t xml:space="preserve">total_adult_poc</t>
+    <t xml:space="preserve">pop_adult_poc</t>
   </si>
   <si>
-    <t xml:space="preserve">total_adult_male_poc</t>
+    <t xml:space="preserve">pop_adult_male_poc</t>
   </si>
   <si>
-    <t xml:space="preserve">total_adult_female_poc</t>
+    <t xml:space="preserve">pop_adult_female_poc</t>
   </si>
   <si>
-    <t xml:space="preserve">total_poc_young</t>
+    <t xml:space="preserve">pop_young_poc</t>
   </si>
   <si>
-    <t xml:space="preserve">total_poc_middle</t>
+    <t xml:space="preserve">pop_middle_poc</t>
   </si>
   <si>
-    <t xml:space="preserve">total_poc_older</t>
+    <t xml:space="preserve">pop_older_poc</t>
   </si>
   <si>
     <t xml:space="preserve">pop_total_hispanic_any_race</t>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">pop_adult_female_hispanic_any_race</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_hispanic_young_any_race</t>
+    <t xml:space="preserve">pop_young_hispanic_any_race</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_hispanic_middle_any_race</t>
+    <t xml:space="preserve">pop_middle_hispanic_any_race</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_hispanic_older_any_race</t>
+    <t xml:space="preserve">pop_older_hispanic_any_race</t>
   </si>
   <si>
     <t xml:space="preserve">pop_total_black_non_hispanic</t>
@@ -98,13 +98,13 @@
     <t xml:space="preserve">pop_adult_female_black_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_black_young_non_hispanic</t>
+    <t xml:space="preserve">pop_young_black_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_black_middle_non_hispanic</t>
+    <t xml:space="preserve">pop_middle_black_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_black_older_non_hispanic</t>
+    <t xml:space="preserve">pop_older_black_non_hispanic</t>
   </si>
   <si>
     <t xml:space="preserve">pop_total_white_non_hispanic</t>
@@ -119,13 +119,13 @@
     <t xml:space="preserve">pop_adult_female_white_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_white_young_non_hispanic</t>
+    <t xml:space="preserve">pop_young_white_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_white_middle_non_hispanic</t>
+    <t xml:space="preserve">pop_middle_white_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_white_older_non_hispanic</t>
+    <t xml:space="preserve">pop_older_white_non_hispanic</t>
   </si>
   <si>
     <t xml:space="preserve">pop_total_AIAN_non_hispanic</t>
@@ -140,13 +140,13 @@
     <t xml:space="preserve">pop_adult_female_AIAN_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_AIAN_young_non_hispanic</t>
+    <t xml:space="preserve">pop_young_AIAN_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_AIAN_middle_non_hispanic</t>
+    <t xml:space="preserve">pop_middle_AIAN_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_AIAN_older_non_hispanic</t>
+    <t xml:space="preserve">pop_older_AIAN_non_hispanic</t>
   </si>
   <si>
     <t xml:space="preserve">pop_total_API_non_hispanic</t>
@@ -161,13 +161,13 @@
     <t xml:space="preserve">pop_adult_female_API_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_API_young_non_hispanic</t>
+    <t xml:space="preserve">pop_young_API_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_API_middle_non_hispanic</t>
+    <t xml:space="preserve">pop_middle_API_non_hispanic</t>
   </si>
   <si>
-    <t xml:space="preserve">pop_API_older_non_hispanic</t>
+    <t xml:space="preserve">pop_older_API_non_hispanic</t>
   </si>
   <si>
     <t xml:space="preserve">04019</t>

</xml_diff>